<commit_message>
dcm and pgm commit on 20230918
</commit_message>
<xml_diff>
--- a/01.管理/WBS.xlsx
+++ b/01.管理/WBS.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1959" documentId="11_31802F1733C7A0836B02CE998FF0545B5A7B8396" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58DE109A-B6A3-489E-A115-CBFC8140CD15}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micch\OneDrive\デスクトップ\PGP\01.管理\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13212"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -93,13 +97,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -454,26 +465,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B565508-1682-4CFC-A7D0-3E0FE297793E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="7" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,12 +507,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -518,7 +529,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -538,12 +549,12 @@
         <v>45060</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -554,14 +565,14 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -574,7 +585,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -587,7 +598,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -600,7 +611,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -613,7 +624,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -626,20 +637,20 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -652,7 +663,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -665,7 +676,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -678,7 +689,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -691,23 +702,24 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="2">
-        <v>45001</v>
+        <v>45194</v>
       </c>
       <c r="E21" s="2">
-        <v>45002</v>
+        <v>45194</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WBS Update commit on 20230924
</commit_message>
<xml_diff>
--- a/01.管理/WBS.xlsx
+++ b/01.管理/WBS.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="WBS" sheetId="5" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WBS!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>作業</t>
   </si>
@@ -70,9 +73,6 @@
     <t>基本・詳細設計</t>
   </si>
   <si>
-    <t>　システム概要書作成</t>
-  </si>
-  <si>
     <t>詳細設計書作成</t>
   </si>
   <si>
@@ -82,9 +82,6 @@
     <t>エネミー</t>
   </si>
   <si>
-    <t>ステージ</t>
-  </si>
-  <si>
     <t>アイテム</t>
   </si>
   <si>
@@ -92,12 +89,63 @@
   </si>
   <si>
     <t>リリース</t>
+  </si>
+  <si>
+    <t>画面定義書作成</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>テイギショ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フィールド</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BGM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コンフィグ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コンフィグ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tasaka・nagata</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tasaka</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>nagata</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>手順書</t>
+    <rPh sb="0" eb="3">
+      <t>テジュンショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,17 +188,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -477,11 +528,8 @@
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.8984375" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" customWidth="1"/>
-    <col min="5" max="5" width="11.09765625" customWidth="1"/>
-    <col min="6" max="6" width="10.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -511,21 +559,28 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4">
         <v>45031</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>45046</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>45031</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>45046</v>
       </c>
     </row>
@@ -536,190 +591,359 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4">
         <v>45047</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>45061</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>45047</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>45060</v>
       </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45122</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45157</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45123</v>
+      </c>
+      <c r="E10" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45162</v>
+      </c>
+      <c r="G10" s="4">
+        <v>45179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45123</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45153</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="4">
+        <v>45123</v>
+      </c>
+      <c r="E12" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45153</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4">
+        <v>45123</v>
+      </c>
+      <c r="E13" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F13" s="4">
+        <v>45179</v>
+      </c>
+      <c r="G13" s="4">
+        <v>45184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4">
+        <v>45123</v>
+      </c>
+      <c r="E14" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F14" s="4">
+        <v>45153</v>
+      </c>
+      <c r="G14" s="4">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4">
         <v>45062</v>
       </c>
-      <c r="E7" s="2">
-        <v>45122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45123</v>
-      </c>
-      <c r="E9" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
+      <c r="E17" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F17" s="4">
+        <v>45135</v>
+      </c>
+      <c r="G17" s="4">
+        <v>45145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2">
-        <v>45123</v>
-      </c>
-      <c r="E10" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E18" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F18" s="4">
+        <v>45062</v>
+      </c>
+      <c r="G18" s="4">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E19" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F19" s="4">
+        <v>45062</v>
+      </c>
+      <c r="G19" s="4">
+        <v>45133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2">
-        <v>45123</v>
-      </c>
-      <c r="E11" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45123</v>
-      </c>
-      <c r="E12" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E20" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F20" s="4">
+        <v>45143</v>
+      </c>
+      <c r="G20" s="4">
+        <v>45148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E21" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F21" s="4">
+        <v>45117</v>
+      </c>
+      <c r="G21" s="4">
+        <v>45148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="4">
+        <v>45062</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45170</v>
+      </c>
+      <c r="F22" s="4">
+        <v>45131</v>
+      </c>
+      <c r="G22" s="4">
+        <v>45184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4">
+        <v>45170</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45189</v>
+      </c>
+      <c r="F24" s="4">
+        <v>45189</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2">
-        <v>45123</v>
-      </c>
-      <c r="E13" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2">
-        <v>45062</v>
-      </c>
-      <c r="E16" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45062</v>
-      </c>
-      <c r="E17" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="2">
-        <v>45062</v>
-      </c>
-      <c r="E18" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45062</v>
-      </c>
-      <c r="E19" s="2">
-        <v>45170</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="D26" s="4">
         <v>45194</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E26" s="4">
         <v>45194</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>